<commit_message>
Updated BOM, PCB files, example, and laser cut file
Add QWIIC and SPI connector cutouts to laser file
</commit_message>
<xml_diff>
--- a/Electrical/miniBCS-4_J005904.xlsx
+++ b/Electrical/miniBCS-4_J005904.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawtelles\Documents\GitHub\miniBSC-4\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB4561C-47D6-43F8-9354-C591CB087DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C57F6CF-8BA7-4C58-9A36-0193E1BE2BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="705" windowWidth="32655" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6780" yWindow="615" windowWidth="30225" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="J005904_miniBCSrevG" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">J005904_miniBCSrevG!$A$1:$J$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">J005904_miniBCSrevG!$A$1:$J$56</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="225">
   <si>
     <t>Qty</t>
   </si>
@@ -694,6 +694,21 @@
   </si>
   <si>
     <t>455-SM04B-SRSS-TBCT-ND</t>
+  </si>
+  <si>
+    <t>IC BUF NON-INVERT 5.5V SOT23-6</t>
+  </si>
+  <si>
+    <t>2ch buffers</t>
+  </si>
+  <si>
+    <t>SN74LVC2G17DBVR</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>296-SN74LVC2G17DBVRCT-ND</t>
   </si>
 </sst>
 </file>
@@ -1246,9 +1261,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1286,7 +1301,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1392,7 +1407,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1534,7 +1549,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1545,10 +1560,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2473,7 +2488,7 @@
         <v>0.87</v>
       </c>
       <c r="J30" s="3">
-        <f t="shared" ref="J30:J50" si="12">A30*I30</f>
+        <f t="shared" ref="J30:J51" si="12">A30*I30</f>
         <v>0.87</v>
       </c>
     </row>
@@ -2869,57 +2884,84 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>221</v>
+      </c>
+      <c r="C48" t="s">
+        <v>220</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H48" t="s">
+        <v>224</v>
+      </c>
+      <c r="I48" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="J48" s="3">
+        <f t="shared" si="12"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>1</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>193</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I50" s="3">
         <v>21.98</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J50" s="3">
         <f t="shared" si="12"/>
         <v>21.98</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>2</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>192</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I51" s="3">
         <v>1.35</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J51" s="3">
         <f t="shared" si="12"/>
         <v>2.7</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J55" s="3">
-        <f>SUM(J4:J51)</f>
-        <v>281.61</v>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J56" s="3">
+        <f>SUM(J4:J52)</f>
+        <v>282.41000000000003</v>
       </c>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="59" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup scale="55" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>